<commit_message>
Adding folder for make_setup.py
Signed-off-by: Rohan <rohan9969@gmail.com>
</commit_message>
<xml_diff>
--- a/Gila_Breath_Camp/Documents/algo_make_setup.xlsx
+++ b/Gila_Breath_Camp/Documents/algo_make_setup.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="27">
   <si>
     <t>folders</t>
   </si>
   <si>
-    <t>files</t>
-  </si>
-  <si>
     <t>folder1</t>
   </si>
   <si>
@@ -99,6 +96,15 @@
   </si>
   <si>
     <t>folder\folder2\folder4\folder6</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>FOLDER</t>
+  </si>
+  <si>
+    <t>TEXT</t>
   </si>
 </sst>
 </file>
@@ -114,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +163,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -196,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -207,6 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="A1:E10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,147 +549,273 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="B15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>3</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
+      <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>3</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added folder 'folder' for make_setup.py testing
Signed-off-by: Rohan <rohan9969@gmail.com>
</commit_message>
<xml_diff>
--- a/Gila_Breath_Camp/Documents/algo_make_setup.xlsx
+++ b/Gila_Breath_Camp/Documents/algo_make_setup.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="27">
-  <si>
-    <t>folders</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
   <si>
     <t>folder1</t>
   </si>
@@ -89,9 +86,6 @@
     <t>folder\folder2</t>
   </si>
   <si>
-    <t>folder\folder2\folder3</t>
-  </si>
-  <si>
     <t>folder\folder2\folder4\folder5</t>
   </si>
   <si>
@@ -105,6 +99,15 @@
   </si>
   <si>
     <t>TEXT</t>
+  </si>
+  <si>
+    <t>folder\folder2\folder4</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>file_name</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,21 +550,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -569,19 +574,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -589,16 +594,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -606,16 +611,16 @@
         <v>0</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -623,16 +628,16 @@
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -640,16 +645,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -657,16 +662,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -674,16 +679,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -691,16 +696,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -708,16 +713,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -725,16 +730,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -742,16 +747,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -759,16 +764,16 @@
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -776,16 +781,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -793,16 +798,16 @@
         <v>3</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="D15" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -810,12 +815,12 @@
         <v>3</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>